<commit_message>
[RowConcealer] add new service "RowConcealer" to hide rows
</commit_message>
<xml_diff>
--- a/tests/data/template.xlsx
+++ b/tests/data/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>%foo%</t>
   </si>
@@ -33,6 +33,10 @@
   </si>
   <si>
     <t>this row remains</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>this row will be hidden</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -381,10 +385,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -410,6 +414,11 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ColumnConcealer] add new service "ColumnConcealer" to hide columns
</commit_message>
<xml_diff>
--- a/tests/data/template.xlsx
+++ b/tests/data/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>%foo%</t>
   </si>
@@ -37,6 +37,30 @@
   </si>
   <si>
     <t>this row will be hidden</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>this</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>col</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>will</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>be</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hidden</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>remains</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -385,10 +409,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -396,29 +420,53 @@
     <col min="1" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ColumnRemover] add new service ColumnRemover
</commit_message>
<xml_diff>
--- a/tests/data/template.xlsx
+++ b/tests/data/template.xlsx
@@ -16,52 +16,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>%foo%</t>
   </si>
   <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>this row will be deleted</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>this row will be deleted - 2</t>
+  </si>
+  <si>
+    <t>will</t>
+  </si>
+  <si>
+    <t>remains</t>
+  </si>
+  <si>
+    <t>this row remains</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>this row will be hidden</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
     <t>hoge</t>
-  </si>
-  <si>
-    <t>this row will be deleted</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>this row will be deleted - 2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>this row remains</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>this row will be hidden</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>this</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>col</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>will</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>be</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>hidden</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>remains</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -409,11 +402,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
@@ -424,49 +415,81 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
       </c>
       <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
         <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -494,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>